<commit_message>
analisi exponential e lognormal
</commit_message>
<xml_diff>
--- a/analysis/dataAnalysis.xlsx
+++ b/analysis/dataAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABB71C7-9B16-4AB2-897E-E7415787125B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638937DC-0188-47C5-BB79-E4D124EDC5D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3564" yWindow="1968" windowWidth="17280" windowHeight="10044" xr2:uid="{B2331E54-D72B-4BDA-A86B-A3C561CB7F3E}"/>
+    <workbookView minimized="1" xWindow="4716" yWindow="60" windowWidth="17280" windowHeight="10044" xr2:uid="{B2331E54-D72B-4BDA-A86B-A3C561CB7F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="48">
   <si>
     <t>count</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>QueueLength</t>
+  </si>
+  <si>
+    <t>EXPONENTIAL</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7382C9-0EF3-45B4-98D4-2E47F47698FB}">
-  <dimension ref="A2:M36"/>
+  <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,43 +727,43 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="B13">
-        <v>0.12633036979032899</v>
+        <v>1.43541988915611E-2</v>
       </c>
       <c r="C13">
-        <v>5.6522920638825899E-3</v>
+        <v>1.91499318904095E-3</v>
       </c>
       <c r="D13">
-        <v>0.11328852119959</v>
+        <v>9.2544316996871993E-3</v>
       </c>
       <c r="E13">
-        <v>0.12235410799249399</v>
+        <v>1.30514059451847E-2</v>
       </c>
       <c r="F13">
-        <v>0.12605540585826</v>
+        <v>1.4223185503462001E-2</v>
       </c>
       <c r="G13">
-        <v>0.13008747269146501</v>
+        <v>1.55180065091397E-2</v>
       </c>
       <c r="H13">
-        <v>0.135005318314256</v>
+        <v>1.7733729684185202E-2</v>
       </c>
       <c r="I13">
-        <v>0.14416688127735999</v>
+        <v>2.0917849898580001E-2</v>
       </c>
       <c r="J13">
-        <v>0.12522252054580801</v>
+        <v>1.4235506384011901E-2</v>
       </c>
       <c r="K13">
-        <v>0.12743821903485</v>
+        <v>1.44728913991102E-2</v>
       </c>
       <c r="L13">
-        <v>0.12487207843784701</v>
+        <v>1.4197960794889299E-2</v>
       </c>
       <c r="M13">
-        <v>0.12778866114281101</v>
+        <v>1.45104369882329E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -878,43 +881,43 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>99</v>
+        <v>1000</v>
       </c>
       <c r="B24">
-        <v>3.2018676494157197E-2</v>
+        <v>3.1885229642875698E-2</v>
       </c>
       <c r="C24">
-        <v>2.7488562167460699E-3</v>
+        <v>2.7156645893726202E-3</v>
       </c>
       <c r="D24">
-        <v>2.5242363270532E-2</v>
+        <v>2.4205202312139001E-2</v>
       </c>
       <c r="E24">
-        <v>3.03030392828555E-2</v>
+        <v>3.01249596508767E-2</v>
       </c>
       <c r="F24">
-        <v>3.1949458483755001E-2</v>
+        <v>3.1702753412856999E-2</v>
       </c>
       <c r="G24">
-        <v>3.3612694937797498E-2</v>
+        <v>3.34688535547885E-2</v>
       </c>
       <c r="H24">
-        <v>3.6690336839077797E-2</v>
+        <v>3.6899804000927197E-2</v>
       </c>
       <c r="I24">
-        <v>3.9837110481586002E-2</v>
+        <v>4.1956793429745003E-2</v>
       </c>
       <c r="J24">
-        <v>3.1477186422635299E-2</v>
+        <v>3.17169110077914E-2</v>
       </c>
       <c r="K24">
-        <v>3.2560166565678998E-2</v>
+        <v>3.2053548277960003E-2</v>
       </c>
       <c r="L24">
-        <v>3.1305898746949799E-2</v>
+        <v>3.1663667357917799E-2</v>
       </c>
       <c r="M24">
-        <v>3.2731454241364498E-2</v>
+        <v>3.2106791927833597E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1016,43 +1019,43 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="B30">
-        <v>1.44514665845502E-2</v>
+        <v>0.12518629139788001</v>
       </c>
       <c r="C30">
-        <v>1.9091167051980399E-3</v>
+        <v>6.1098483936431799E-3</v>
       </c>
       <c r="D30">
-        <v>9.8730606488011009E-3</v>
+        <v>0.10956655552706</v>
       </c>
       <c r="E30">
-        <v>1.3130214967730499E-2</v>
+        <v>0.120789937824345</v>
       </c>
       <c r="F30">
-        <v>1.44878022986265E-2</v>
+        <v>0.124878148431015</v>
       </c>
       <c r="G30">
-        <v>1.5666003173531701E-2</v>
+        <v>0.12894825212483699</v>
       </c>
       <c r="H30">
-        <v>1.73407299861459E-2</v>
+        <v>0.13572442178319</v>
       </c>
       <c r="I30">
-        <v>1.9855823953459001E-2</v>
+        <v>0.14572280329442999</v>
       </c>
       <c r="J30">
-        <v>1.4077279710331301E-2</v>
+        <v>0.124807599071068</v>
       </c>
       <c r="K30">
-        <v>1.4825653458769E-2</v>
+        <v>0.12556498372469099</v>
       </c>
       <c r="L30">
-        <v>1.39589144746091E-2</v>
+        <v>0.124687808641158</v>
       </c>
       <c r="M30">
-        <v>1.4944018694491299E-2</v>
+        <v>0.125684774154601</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1060,7 +1063,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1.96</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>85.073494809688569</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -1091,12 +1094,497 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0.05</v>
       </c>
       <c r="B36">
         <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43">
+        <v>8.4892330083718246E-3</v>
+      </c>
+      <c r="F43">
+        <v>8.5180645917998996E-3</v>
+      </c>
+      <c r="G43">
+        <v>8.5506116118631743E-3</v>
+      </c>
+      <c r="H43">
+        <v>8.5995810192785408E-3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1000</v>
+      </c>
+      <c r="B50">
+        <v>1.43541988915611E-2</v>
+      </c>
+      <c r="C50">
+        <v>1.91499318904095E-3</v>
+      </c>
+      <c r="D50">
+        <v>9.2544316996871993E-3</v>
+      </c>
+      <c r="E50">
+        <v>1.30514059451847E-2</v>
+      </c>
+      <c r="F50">
+        <v>1.4223185503462001E-2</v>
+      </c>
+      <c r="G50">
+        <v>1.55180065091397E-2</v>
+      </c>
+      <c r="H50">
+        <v>1.7733729684185202E-2</v>
+      </c>
+      <c r="I50">
+        <v>2.0917849898580001E-2</v>
+      </c>
+      <c r="J50">
+        <v>1.4235506384011901E-2</v>
+      </c>
+      <c r="K50">
+        <v>1.44728913991102E-2</v>
+      </c>
+      <c r="L50">
+        <v>1.4197960794889299E-2</v>
+      </c>
+      <c r="M50">
+        <v>1.45104369882329E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59">
+        <v>8.8826554990601003E-3</v>
+      </c>
+      <c r="F59">
+        <v>8.9180535757102004E-3</v>
+      </c>
+      <c r="G59">
+        <v>8.95210542649315E-3</v>
+      </c>
+      <c r="H59">
+        <v>9.0081783547581503E-3</v>
+      </c>
+      <c r="I59" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" t="s">
+        <v>28</v>
+      </c>
+      <c r="K59" t="s">
+        <v>29</v>
+      </c>
+      <c r="L59" t="s">
+        <v>30</v>
+      </c>
+      <c r="M59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>10000</v>
+      </c>
+      <c r="B61">
+        <v>2.80564496878336E-2</v>
+      </c>
+      <c r="C61">
+        <v>7.8403553352260902E-3</v>
+      </c>
+      <c r="D61">
+        <v>5.9582919563059E-3</v>
+      </c>
+      <c r="E61">
+        <v>2.257636122178E-2</v>
+      </c>
+      <c r="F61">
+        <v>2.7397260273973E-2</v>
+      </c>
+      <c r="G61">
+        <v>3.27324042520395E-2</v>
+      </c>
+      <c r="H61">
+        <v>4.1846616629692003E-2</v>
+      </c>
+      <c r="I61">
+        <v>7.3710073710074001E-2</v>
+      </c>
+      <c r="J61">
+        <v>2.7902778723263199E-2</v>
+      </c>
+      <c r="K61">
+        <v>2.8210120652404001E-2</v>
+      </c>
+      <c r="L61">
+        <v>2.78541685201848E-2</v>
+      </c>
+      <c r="M61">
+        <v>2.8258730855482399E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65">
+        <v>1.0248790207165251E-2</v>
+      </c>
+      <c r="F65">
+        <v>1.03047904810325E-2</v>
+      </c>
+      <c r="G65">
+        <v>1.0355157586976999E-2</v>
+      </c>
+      <c r="H65">
+        <v>1.04478342129787E-2</v>
+      </c>
+      <c r="I65" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K65" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" t="s">
+        <v>38</v>
+      </c>
+      <c r="M65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>10000</v>
+      </c>
+      <c r="B67">
+        <v>0.107514171139015</v>
+      </c>
+      <c r="C67">
+        <v>1.6694440292773699E-2</v>
+      </c>
+      <c r="D67">
+        <v>5.1546391752576998E-2</v>
+      </c>
+      <c r="E67">
+        <v>9.5953091174636199E-2</v>
+      </c>
+      <c r="F67">
+        <v>0.106428086744965</v>
+      </c>
+      <c r="G67">
+        <v>0.11783331628938699</v>
+      </c>
+      <c r="H67">
+        <v>0.13656647462962099</v>
+      </c>
+      <c r="I67">
+        <v>0.22504047490556001</v>
+      </c>
+      <c r="J67">
+        <v>0.107186960109277</v>
+      </c>
+      <c r="K67">
+        <v>0.107841382168754</v>
+      </c>
+      <c r="L67">
+        <v>0.107083454579462</v>
+      </c>
+      <c r="M67">
+        <v>0.107944887698569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lognormal ed exponential analysis
</commit_message>
<xml_diff>
--- a/analysis/dataAnalysis.xlsx
+++ b/analysis/dataAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638937DC-0188-47C5-BB79-E4D124EDC5D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E2B9C4-DDDF-4508-ACF5-C927F95FB936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4716" yWindow="60" windowWidth="17280" windowHeight="10044" xr2:uid="{B2331E54-D72B-4BDA-A86B-A3C561CB7F3E}"/>
+    <workbookView xWindow="4680" yWindow="2736" windowWidth="17280" windowHeight="10044" xr2:uid="{B2331E54-D72B-4BDA-A86B-A3C561CB7F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
   <si>
     <t>count</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>EXPONENTIAL</t>
+  </si>
+  <si>
+    <t>LOGNORMAL</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -246,11 +249,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -260,6 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7382C9-0EF3-45B4-98D4-2E47F47698FB}">
-  <dimension ref="A2:M67"/>
+  <dimension ref="A2:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,7 +894,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1013,7 +1032,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1159,44 +1178,44 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
+      <c r="A43">
+        <v>905</v>
+      </c>
+      <c r="B43">
+        <v>7.8725696302850597E-3</v>
+      </c>
+      <c r="C43">
+        <v>1.9488603207600799E-4</v>
+      </c>
+      <c r="D43">
+        <v>7.1938752625625001E-3</v>
       </c>
       <c r="E43">
-        <v>8.4892330083718246E-3</v>
+        <v>7.7643529690939999E-3</v>
       </c>
       <c r="F43">
-        <v>8.5180645917998996E-3</v>
+        <v>7.8601528898132999E-3</v>
       </c>
       <c r="G43">
-        <v>8.5506116118631743E-3</v>
+        <v>7.9617084655649994E-3</v>
       </c>
       <c r="H43">
-        <v>8.5995810192785408E-3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" t="s">
-        <v>19</v>
-      </c>
-      <c r="K43" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" t="s">
-        <v>21</v>
-      </c>
-      <c r="M43" t="s">
-        <v>22</v>
+        <v>8.1675895685990804E-3</v>
+      </c>
+      <c r="I43">
+        <v>9.7404068141463008E-3</v>
+      </c>
+      <c r="J43">
+        <v>7.8598722977066791E-3</v>
+      </c>
+      <c r="K43">
+        <v>7.8852669628634402E-3</v>
+      </c>
+      <c r="L43">
+        <v>7.8558557945441303E-3</v>
+      </c>
+      <c r="M43">
+        <v>7.8892834660259908E-3</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -1236,61 +1255,47 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A49">
         <v>1000</v>
       </c>
-      <c r="B50">
-        <v>1.43541988915611E-2</v>
-      </c>
-      <c r="C50">
-        <v>1.91499318904095E-3</v>
-      </c>
-      <c r="D50">
-        <v>9.2544316996871993E-3</v>
-      </c>
-      <c r="E50">
-        <v>1.30514059451847E-2</v>
-      </c>
-      <c r="F50">
-        <v>1.4223185503462001E-2</v>
-      </c>
-      <c r="G50">
-        <v>1.55180065091397E-2</v>
-      </c>
-      <c r="H50">
-        <v>1.7733729684185202E-2</v>
-      </c>
-      <c r="I50">
-        <v>2.0917849898580001E-2</v>
-      </c>
-      <c r="J50">
-        <v>1.4235506384011901E-2</v>
-      </c>
-      <c r="K50">
-        <v>1.44728913991102E-2</v>
-      </c>
-      <c r="L50">
-        <v>1.4197960794889299E-2</v>
-      </c>
-      <c r="M50">
-        <v>1.45104369882329E-2</v>
-      </c>
-    </row>
+      <c r="B49">
+        <v>1.2835977960860299E-2</v>
+      </c>
+      <c r="C49">
+        <v>5.5386968329972997E-3</v>
+      </c>
+      <c r="D49">
+        <v>1.6155088852989E-3</v>
+      </c>
+      <c r="E49">
+        <v>9.04831222888677E-3</v>
+      </c>
+      <c r="F49">
+        <v>1.2104705981471999E-2</v>
+      </c>
+      <c r="G49">
+        <v>1.5904572564611998E-2</v>
+      </c>
+      <c r="H49">
+        <v>2.2772304768601901E-2</v>
+      </c>
+      <c r="I49">
+        <v>3.9237668161435001E-2</v>
+      </c>
+      <c r="J49">
+        <v>1.24926859745362E-2</v>
+      </c>
+      <c r="K49">
+        <v>1.3179269947184401E-2</v>
+      </c>
+      <c r="L49">
+        <v>1.23840936115154E-2</v>
+      </c>
+      <c r="M49">
+        <v>1.32878623102053E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>9</v>
@@ -1363,90 +1368,90 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" t="s">
-        <v>26</v>
+      <c r="A59">
+        <v>917</v>
+      </c>
+      <c r="B59">
+        <v>8.2262451841476E-3</v>
+      </c>
+      <c r="C59">
+        <v>2.6277268534421198E-4</v>
+      </c>
+      <c r="D59">
+        <v>7.3125575348333E-3</v>
       </c>
       <c r="E59">
-        <v>8.8826554990601003E-3</v>
+        <v>8.0856696115783003E-3</v>
       </c>
       <c r="F59">
-        <v>8.9180535757102004E-3</v>
+        <v>8.1977956593076006E-3</v>
       </c>
       <c r="G59">
-        <v>8.95210542649315E-3</v>
+        <v>8.3288008162528994E-3</v>
       </c>
       <c r="H59">
-        <v>9.0081783547581503E-3</v>
-      </c>
-      <c r="I59" t="s">
-        <v>27</v>
-      </c>
-      <c r="J59" t="s">
-        <v>28</v>
-      </c>
-      <c r="K59" t="s">
-        <v>29</v>
-      </c>
-      <c r="L59" t="s">
-        <v>30</v>
-      </c>
-      <c r="M59" t="s">
-        <v>31</v>
+        <v>8.6265968194983791E-3</v>
+      </c>
+      <c r="I59">
+        <v>1.0357827646121E-2</v>
+      </c>
+      <c r="J59">
+        <v>8.2092372477628999E-3</v>
+      </c>
+      <c r="K59">
+        <v>8.2432531205323002E-3</v>
+      </c>
+      <c r="L59">
+        <v>8.2038571862534503E-3</v>
+      </c>
+      <c r="M59">
+        <v>8.2486331820417497E-3</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="B61">
-        <v>2.80564496878336E-2</v>
+        <v>2.82476371266644E-2</v>
       </c>
       <c r="C61">
-        <v>7.8403553352260902E-3</v>
+        <v>7.9296935880219504E-3</v>
       </c>
       <c r="D61">
-        <v>5.9582919563059E-3</v>
+        <v>9.5465393794748991E-3</v>
       </c>
       <c r="E61">
-        <v>2.257636122178E-2</v>
+        <v>2.2900763358779001E-2</v>
       </c>
       <c r="F61">
-        <v>2.7397260273973E-2</v>
+        <v>2.7612535694817E-2</v>
       </c>
       <c r="G61">
-        <v>3.27324042520395E-2</v>
+        <v>3.2942357044153499E-2</v>
       </c>
       <c r="H61">
-        <v>4.1846616629692003E-2</v>
+        <v>4.2352853835009897E-2</v>
       </c>
       <c r="I61">
-        <v>7.3710073710074001E-2</v>
+        <v>6.1769616026711001E-2</v>
       </c>
       <c r="J61">
-        <v>2.7902778723263199E-2</v>
+        <v>2.77561496261109E-2</v>
       </c>
       <c r="K61">
-        <v>2.8210120652404001E-2</v>
+        <v>2.87391246272179E-2</v>
       </c>
       <c r="L61">
-        <v>2.78541685201848E-2</v>
+        <v>2.7600679090221601E-2</v>
       </c>
       <c r="M61">
-        <v>2.8258730855482399E-2</v>
+        <v>2.8894595163107301E-2</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -1501,90 +1506,575 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" t="s">
-        <v>33</v>
-      </c>
-      <c r="D65" t="s">
-        <v>34</v>
+      <c r="A65">
+        <v>904</v>
+      </c>
+      <c r="B65">
+        <v>9.3402780566278001E-3</v>
+      </c>
+      <c r="C65">
+        <v>4.6752278633720298E-4</v>
+      </c>
+      <c r="D65">
+        <v>8.1237281397447004E-3</v>
       </c>
       <c r="E65">
-        <v>1.0248790207165251E-2</v>
+        <v>9.1428105672243503E-3</v>
       </c>
       <c r="F65">
-        <v>1.03047904810325E-2</v>
+        <v>9.2998227869489497E-3</v>
       </c>
       <c r="G65">
-        <v>1.0355157586976999E-2</v>
+        <v>9.4707697553082192E-3</v>
       </c>
       <c r="H65">
-        <v>1.04478342129787E-2</v>
-      </c>
-      <c r="I65" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65" t="s">
-        <v>36</v>
-      </c>
-      <c r="K65" t="s">
-        <v>37</v>
-      </c>
-      <c r="L65" t="s">
-        <v>38</v>
-      </c>
-      <c r="M65" t="s">
-        <v>39</v>
+        <v>9.9089177903067295E-3</v>
+      </c>
+      <c r="I65">
+        <v>1.5026117763905E-2</v>
+      </c>
+      <c r="J65">
+        <v>9.3098008865462201E-3</v>
+      </c>
+      <c r="K65">
+        <v>9.3707552267093801E-3</v>
+      </c>
+      <c r="L65">
+        <v>9.3001601490714392E-3</v>
+      </c>
+      <c r="M65">
+        <v>9.3803959641841697E-3</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="B67">
-        <v>0.107514171139015</v>
+        <v>0.108256090055896</v>
       </c>
       <c r="C67">
-        <v>1.6694440292773699E-2</v>
+        <v>1.6907935759690899E-2</v>
       </c>
       <c r="D67">
-        <v>5.1546391752576998E-2</v>
+        <v>5.5721393034825997E-2</v>
       </c>
       <c r="E67">
-        <v>9.5953091174636199E-2</v>
+        <v>9.66293995987417E-2</v>
       </c>
       <c r="F67">
-        <v>0.106428086744965</v>
+        <v>0.10656194721064401</v>
       </c>
       <c r="G67">
-        <v>0.11783331628938699</v>
+        <v>0.11808774493985701</v>
       </c>
       <c r="H67">
-        <v>0.13656647462962099</v>
+        <v>0.13823229730028799</v>
       </c>
       <c r="I67">
-        <v>0.22504047490556001</v>
+        <v>0.17809096732863999</v>
       </c>
       <c r="J67">
-        <v>0.107186960109277</v>
+        <v>0.107208125340261</v>
       </c>
       <c r="K67">
-        <v>0.107841382168754</v>
+        <v>0.109304054771532</v>
       </c>
       <c r="L67">
-        <v>0.107083454579462</v>
+        <v>0.10687662629756001</v>
       </c>
       <c r="M67">
-        <v>0.107944887698569</v>
+        <v>0.109635553814233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F73" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>905</v>
+      </c>
+      <c r="B74">
+        <v>7.8725696302850597E-3</v>
+      </c>
+      <c r="C74">
+        <v>1.9488603207600799E-4</v>
+      </c>
+      <c r="D74">
+        <v>7.1938752625625001E-3</v>
+      </c>
+      <c r="E74">
+        <v>7.7643529690939999E-3</v>
+      </c>
+      <c r="F74">
+        <v>7.8601528898132999E-3</v>
+      </c>
+      <c r="G74">
+        <v>7.9617084655649994E-3</v>
+      </c>
+      <c r="H74">
+        <v>8.1675895685990804E-3</v>
+      </c>
+      <c r="I74">
+        <v>9.7404068141463008E-3</v>
+      </c>
+      <c r="J74">
+        <v>7.8598722977066791E-3</v>
+      </c>
+      <c r="K74">
+        <v>7.8852669628634402E-3</v>
+      </c>
+      <c r="L74">
+        <v>7.8558557945441303E-3</v>
+      </c>
+      <c r="M74">
+        <v>7.8892834660259908E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="8"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>905</v>
+      </c>
+      <c r="B80">
+        <v>1.2375246763944201E-2</v>
+      </c>
+      <c r="C80">
+        <v>1.08004558234438E-2</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>7.7120822622108003E-3</v>
+      </c>
+      <c r="F80">
+        <v>1.1578541103821E-2</v>
+      </c>
+      <c r="G80">
+        <v>1.5477214101462E-2</v>
+      </c>
+      <c r="H80">
+        <v>2.4923592625455501E-2</v>
+      </c>
+      <c r="I80">
+        <v>0.21951219512195</v>
+      </c>
+      <c r="J80">
+        <v>1.1671568936818699E-2</v>
+      </c>
+      <c r="K80">
+        <v>1.30789245910696E-2</v>
+      </c>
+      <c r="L80">
+        <v>1.1448976971095299E-2</v>
+      </c>
+      <c r="M80">
+        <v>1.3301516556793E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G89" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H89" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>917</v>
+      </c>
+      <c r="B90">
+        <v>8.2262451841476E-3</v>
+      </c>
+      <c r="C90">
+        <v>2.6277268534421198E-4</v>
+      </c>
+      <c r="D90">
+        <v>7.3125575348333E-3</v>
+      </c>
+      <c r="E90">
+        <v>8.0856696115783003E-3</v>
+      </c>
+      <c r="F90">
+        <v>8.1977956593076006E-3</v>
+      </c>
+      <c r="G90">
+        <v>8.3288008162528994E-3</v>
+      </c>
+      <c r="H90">
+        <v>8.6265968194983791E-3</v>
+      </c>
+      <c r="I90">
+        <v>1.0357827646121E-2</v>
+      </c>
+      <c r="J90">
+        <v>8.2092372477628999E-3</v>
+      </c>
+      <c r="K90">
+        <v>8.2432531205323002E-3</v>
+      </c>
+      <c r="L90">
+        <v>8.2038571862534503E-3</v>
+      </c>
+      <c r="M90">
+        <v>8.2486331820417497E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>917</v>
+      </c>
+      <c r="B92">
+        <v>2.7967860199466999E-2</v>
+      </c>
+      <c r="C92">
+        <v>1.5918407591378001E-2</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>2.0967741935484001E-2</v>
+      </c>
+      <c r="F92">
+        <v>2.6501035196686999E-2</v>
+      </c>
+      <c r="G92">
+        <v>3.2631578947367998E-2</v>
+      </c>
+      <c r="H92">
+        <v>4.8255582137161399E-2</v>
+      </c>
+      <c r="I92">
+        <v>0.16666666666666999</v>
+      </c>
+      <c r="J92">
+        <v>2.6937542823422801E-2</v>
+      </c>
+      <c r="K92">
+        <v>2.8998177575511201E-2</v>
+      </c>
+      <c r="L92">
+        <v>2.66116261024293E-2</v>
+      </c>
+      <c r="M92">
+        <v>2.9324094296504798E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G95" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H95" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>904</v>
+      </c>
+      <c r="B96">
+        <v>9.3402780566278001E-3</v>
+      </c>
+      <c r="C96">
+        <v>4.6752278633720298E-4</v>
+      </c>
+      <c r="D96">
+        <v>8.1237281397447004E-3</v>
+      </c>
+      <c r="E96">
+        <v>9.1428105672243503E-3</v>
+      </c>
+      <c r="F96">
+        <v>9.2998227869489497E-3</v>
+      </c>
+      <c r="G96">
+        <v>9.4707697553082192E-3</v>
+      </c>
+      <c r="H96">
+        <v>9.9089177903067295E-3</v>
+      </c>
+      <c r="I96">
+        <v>1.5026117763905E-2</v>
+      </c>
+      <c r="J96">
+        <v>9.3098008865462201E-3</v>
+      </c>
+      <c r="K96">
+        <v>9.3707552267093801E-3</v>
+      </c>
+      <c r="L96">
+        <v>9.3001601490714392E-3</v>
+      </c>
+      <c r="M96">
+        <v>9.3803959641841697E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>904</v>
+      </c>
+      <c r="B98">
+        <v>0.10465632307610299</v>
+      </c>
+      <c r="C98">
+        <v>3.48134397648448E-2</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>9.0533753924660995E-2</v>
+      </c>
+      <c r="F98">
+        <v>0.10222843951490999</v>
+      </c>
+      <c r="G98">
+        <v>0.11371127181492401</v>
+      </c>
+      <c r="H98">
+        <v>0.15193924898661501</v>
+      </c>
+      <c r="I98">
+        <v>0.50769230769231</v>
+      </c>
+      <c r="J98">
+        <v>0.10238688262133901</v>
+      </c>
+      <c r="K98">
+        <v>0.106925763530868</v>
+      </c>
+      <c r="L98">
+        <v>0.101668998395852</v>
+      </c>
+      <c r="M98">
+        <v>0.107643647756355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>